<commit_message>
Updated workflow up to plotNormFiring section.
</commit_message>
<xml_diff>
--- a/Documentation/renaming_CRF_ephys_workflow.xlsx
+++ b/Documentation/renaming_CRF_ephys_workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\James\Dropbox (Personal)\Public\Science Data\Sparta Lab\Work in Progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\James\Dropbox (Personal)\Public\Science Data\Sparta Lab\Sparta-Lab-CRF-Ephys-Paper-Scripts-and-Data\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B627B9-4B3E-4DBE-A066-B19094219EB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E06DAD3-B1A7-443D-B7D4-8E8C97E403F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D47C3AF4-5866-4CBD-A858-7AA462BDF272}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="42">
   <si>
     <t>Original Script Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>findOutliers_DATA_RawSpikes_SaveBins_CutLicks</t>
   </si>
   <si>
-    <t>makeUnitTimestampVarsForAll</t>
-  </si>
-  <si>
     <t>BURSTunits_Analysis</t>
   </si>
   <si>
@@ -60,15 +57,9 @@
     <t>nexPrepAll_forNormFiringFigsSplitByDeltaRate</t>
   </si>
   <si>
-    <t>make_variables_for_bursts</t>
-  </si>
-  <si>
     <t>calc_perc_bursts_by_hour</t>
   </si>
   <si>
-    <t>prep_data_for_norm_firing</t>
-  </si>
-  <si>
     <t>nexDATAcountUnitsFinal_v2</t>
   </si>
   <si>
@@ -84,44 +75,95 @@
     <t>Order</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
-    <t>get_data_from_nex_files_with_bursts</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
     <t>import_nex_files_spikes_and_bursts.m</t>
   </si>
   <si>
-    <t>classify_unit_light_lick_types</t>
-  </si>
-  <si>
-    <t>incorporated into import_ nex_files_spikes_and_bursts</t>
-  </si>
-  <si>
-    <t>count_unit_responses_for_table</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>minimal_burst_analysis</t>
-  </si>
-  <si>
-    <t>used new get_unit_index function</t>
+    <t>1B. minimal_burst_analysis</t>
+  </si>
+  <si>
+    <t>3B. count_unit_responses_for_table</t>
+  </si>
+  <si>
+    <t>calculate_light_lick_responses</t>
+  </si>
+  <si>
+    <t>prep_data_for_norm_firing_fig</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saves all units, neurons, intervals into DATA, calculates BURSTunits. Runs Nex templates. </t>
+  </si>
+  <si>
+    <t>Process each unit's timestamps to calssify its lick and light-responsiveness</t>
+  </si>
+  <si>
+    <t>Uses rolling window to calculate outlier-removed binned data. Runs counts_unit_responses_for_table</t>
+  </si>
+  <si>
+    <t>Creates a structure of tables with the count of all light and lick responses.</t>
+  </si>
+  <si>
+    <t>corrSPIKESandLICKSv2_updateMatchV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plotNormFiringFromSORTtracker_V2WIP  plotNormFiringFromSORTtracker_V3WIP </t>
+  </si>
+  <si>
+    <t>printUnitNamesDetailsOutRem</t>
+  </si>
+  <si>
+    <t>copyPasteSORTdata</t>
+  </si>
+  <si>
+    <t>copyPasteSORTdata_EarlyVsLate</t>
+  </si>
+  <si>
+    <t>copyPasteSORTdata_EarlyVsLateSPLITS</t>
+  </si>
+  <si>
+    <t>Calculates normalized firing data and creates structures for color plot</t>
+  </si>
+  <si>
+    <t>Generates normalized firing rate figure</t>
+  </si>
+  <si>
+    <t>calcualtes corerlations between spikes and licks</t>
+  </si>
+  <si>
+    <t>prints out a table of all unit's results</t>
+  </si>
+  <si>
+    <t>Prints out grouped data for Prism/Excel</t>
+  </si>
+  <si>
+    <t>Calcualtes % of spikes in bursts by hour.</t>
+  </si>
+  <si>
+    <t>Run By User</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>SORTtracker=SORTtracker.CRF; SORTtrackerCRF=SORTtracker_SplitByRateChange.CRF</t>
+  </si>
+  <si>
+    <t>USER MUST ENTER MANUALLY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,28 +172,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,9 +225,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,32 +234,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -221,7 +304,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -246,16 +338,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D289FB4-4C17-472A-85A9-ABF39602CC9D}" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E9" xr:uid="{53D6DD0C-B2D0-46CF-A093-42B205A91144}"/>
-  <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{8D7647F2-6793-4883-BE10-614D29E726EB}" name="Order" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D289FB4-4C17-472A-85A9-ABF39602CC9D}" name="Table1" displayName="Table1" ref="B3:G17" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="B3:G17" xr:uid="{53D6DD0C-B2D0-46CF-A093-42B205A91144}"/>
+  <tableColumns count="6">
+    <tableColumn id="4" xr3:uid="{8D7647F2-6793-4883-BE10-614D29E726EB}" name="Order" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6CD1E5BE-BE71-4E46-9B10-B5E7EC7A2E08}" name="Run By User" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{313B8C19-4922-44EC-8300-FC839B889845}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CEB107AC-5D94-4619-B737-91AFD348E2DC}" name="Changed" dataDxfId="1"/>
     <tableColumn id="1" xr3:uid="{A0874E6F-8E55-4E59-8EDD-856191B2FA6A}" name="Original Script Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CEB107AC-5D94-4619-B737-91AFD348E2DC}" name="Changed" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{0D411A09-B4B2-497B-B5A2-CF00FE2ACCB1}" name="WIP" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -556,159 +649,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADC88EB-0D15-4452-9F23-EF3ADCBB57B8}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="B3:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="E10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="7" t="s">
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="6" t="s">
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated scripts up to/partially including pre_data_for_norm_firing_fig
</commit_message>
<xml_diff>
--- a/Documentation/renaming_CRF_ephys_workflow.xlsx
+++ b/Documentation/renaming_CRF_ephys_workflow.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\James\Dropbox (Personal)\Public\Science Data\Sparta Lab\Sparta-Lab-CRF-Ephys-Paper-Scripts-and-Data\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E06DAD3-B1A7-443D-B7D4-8E8C97E403F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476123BE-45AD-4D9D-B0CF-BD0E91B1AE30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D47C3AF4-5866-4CBD-A858-7AA462BDF272}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="script_overview" sheetId="1" r:id="rId1"/>
+    <sheet name="dependency_report" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
   <si>
     <t>Original Script Name</t>
   </si>
@@ -157,23 +159,118 @@
   </si>
   <si>
     <t>USER MUST ENTER MANUALLY</t>
+  </si>
+  <si>
+    <t>File Tested</t>
+  </si>
+  <si>
+    <t>calculate_light_lick_responses.m</t>
+  </si>
+  <si>
+    <t>Required File #1</t>
+  </si>
+  <si>
+    <t>calcWFcorrelationMLTrigd</t>
+  </si>
+  <si>
+    <t>JMI_spkMatFun</t>
+  </si>
+  <si>
+    <t>clearCRFdata</t>
+  </si>
+  <si>
+    <t>cutBinTimesGoodInts</t>
+  </si>
+  <si>
+    <t>Required File #2</t>
+  </si>
+  <si>
+    <t>classify_unit_light_type</t>
+  </si>
+  <si>
+    <t>replaceBinnedOutliers</t>
+  </si>
+  <si>
+    <t>Required File #3</t>
+  </si>
+  <si>
+    <t>get_unit_index</t>
+  </si>
+  <si>
+    <t>cutTimesGoodIntsFast</t>
+  </si>
+  <si>
+    <t>Required File #4</t>
+  </si>
+  <si>
+    <t>remove_nan_rows</t>
+  </si>
+  <si>
+    <t>nexOptionsCriteria</t>
+  </si>
+  <si>
+    <t>calc_spike_binned_data_remove_outliers</t>
+  </si>
+  <si>
+    <t>Required File #5</t>
+  </si>
+  <si>
+    <t>split_cell_array_by_column</t>
+  </si>
+  <si>
+    <t>unit_responses_stat_tests</t>
+  </si>
+  <si>
+    <t>count_unit_responses_for_table</t>
+  </si>
+  <si>
+    <t>Required File #6</t>
+  </si>
+  <si>
+    <t>split_unit_results_header</t>
+  </si>
+  <si>
+    <t>counts2table</t>
+  </si>
+  <si>
+    <t>Required File #7</t>
+  </si>
+  <si>
+    <t>import_nex_files_spikes_and_bursts</t>
+  </si>
+  <si>
+    <t>nexDATA_fillDrinkDay</t>
+  </si>
+  <si>
+    <t>Required File #8</t>
+  </si>
+  <si>
+    <t>minimal_burst_analysis</t>
+  </si>
+  <si>
+    <t>renameDATAfileinfoDrinkTypeDay</t>
+  </si>
+  <si>
+    <t>Required File #9</t>
+  </si>
+  <si>
+    <t>nexCutRateHistoNexTrigdFUN</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>calculate_corr_spikes_bursts_licks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -257,36 +354,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -313,10 +398,22 @@
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -342,11 +439,11 @@
   <autoFilter ref="B3:G17" xr:uid="{53D6DD0C-B2D0-46CF-A093-42B205A91144}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{8D7647F2-6793-4883-BE10-614D29E726EB}" name="Order" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6CD1E5BE-BE71-4E46-9B10-B5E7EC7A2E08}" name="Run By User" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{313B8C19-4922-44EC-8300-FC839B889845}" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6CD1E5BE-BE71-4E46-9B10-B5E7EC7A2E08}" name="Run By User" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{313B8C19-4922-44EC-8300-FC839B889845}" name="Description" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{CEB107AC-5D94-4619-B737-91AFD348E2DC}" name="Changed" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{A0874E6F-8E55-4E59-8EDD-856191B2FA6A}" name="Original Script Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A0874E6F-8E55-4E59-8EDD-856191B2FA6A}" name="Original Script Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -651,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADC88EB-0D15-4452-9F23-EF3ADCBB57B8}">
   <dimension ref="B3:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,30 +910,30 @@
       <c r="C10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
@@ -848,7 +945,9 @@
       <c r="E12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>25</v>
       </c>
@@ -859,6 +958,9 @@
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>32</v>
@@ -935,4 +1037,178 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6697E1-6CC3-4E1C-9A88-E8518BD48519}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E7360B-42FD-4B5F-AF71-007BB8C1704A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All scripts updated, except final copyPaste scripts for Prism figures.
</commit_message>
<xml_diff>
--- a/Documentation/renaming_CRF_ephys_workflow.xlsx
+++ b/Documentation/renaming_CRF_ephys_workflow.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\James\Dropbox (Personal)\Public\Science Data\Sparta Lab\Sparta-Lab-CRF-Ephys-Paper-Scripts-and-Data\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A3D886-49F6-4155-BE48-0AF9AD453301}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2CC4D9-9105-4607-8A5E-E5839080F006}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D47C3AF4-5866-4CBD-A858-7AA462BDF272}"/>
   </bookViews>
   <sheets>
     <sheet name="script_overview" sheetId="1" r:id="rId1"/>
-    <sheet name="dependency_report" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="DATA MAP" sheetId="5" r:id="rId2"/>
+    <sheet name="dependency_report" sheetId="3" r:id="rId3"/>
+    <sheet name="dependency_report05-02" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="98">
   <si>
     <t>Original Script Name</t>
   </si>
@@ -149,15 +151,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
-    <t>SORTtracker=SORTtracker.CRF; SORTtrackerCRF=SORTtracker_SplitByRateChange.CRF</t>
-  </si>
-  <si>
-    <t>USER MUST ENTER MANUALLY</t>
-  </si>
-  <si>
     <t>File Tested</t>
   </si>
   <si>
@@ -254,15 +247,9 @@
     <t>nexCutRateHistoNexTrigdFUN</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>calculate_corr_spikes_bursts_licks</t>
   </si>
   <si>
-    <t>detect_or_fill_drink_day.m</t>
-  </si>
-  <si>
     <t>3B. calc_perc_bursts_by_hour</t>
   </si>
   <si>
@@ -270,13 +257,85 @@
   </si>
   <si>
     <t>print_results_table_to_excel.m</t>
+  </si>
+  <si>
+    <t>rates_table_to_excel</t>
+  </si>
+  <si>
+    <t>detect_or_fill_drink_days</t>
+  </si>
+  <si>
+    <t>Required File #10</t>
+  </si>
+  <si>
+    <t>detect_drink_type_and_day</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>fileinfo</t>
+  </si>
+  <si>
+    <t>make_RATES_structure_and_table.m</t>
+  </si>
+  <si>
+    <t>first half of nexPrepForAll..plus new rates_table_to_excel</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>export firing rates data to excel spreadsheets.</t>
+  </si>
+  <si>
+    <t>Makes RATEScut structure and triggers rates_table_to_excel</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>3E</t>
+  </si>
+  <si>
+    <t>plot_normalized_firing_CRF_by_lick_types.</t>
+  </si>
+  <si>
+    <t>detect_or_fill_drink_day.m / deect_drink_type_and_day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically recognizes drink type and day # from file names. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Separates  nexResults for bursting analysis into BURSTunits structure. </t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>plot_normalized_firing_CRF_by_lick_types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,15 +350,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -314,8 +382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -328,62 +395,107 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -401,36 +513,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -447,15 +553,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D289FB4-4C17-472A-85A9-ABF39602CC9D}" name="Table1" displayName="Table1" ref="B3:G18" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="B3:G18" xr:uid="{53D6DD0C-B2D0-46CF-A093-42B205A91144}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D289FB4-4C17-472A-85A9-ABF39602CC9D}" name="Table1" displayName="Table1" ref="B3:G20" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B3:G20" xr:uid="{53D6DD0C-B2D0-46CF-A093-42B205A91144}"/>
   <tableColumns count="6">
-    <tableColumn id="4" xr3:uid="{8D7647F2-6793-4883-BE10-614D29E726EB}" name="Order" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6CD1E5BE-BE71-4E46-9B10-B5E7EC7A2E08}" name="Run By User" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{313B8C19-4922-44EC-8300-FC839B889845}" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CEB107AC-5D94-4619-B737-91AFD348E2DC}" name="Changed" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{A0874E6F-8E55-4E59-8EDD-856191B2FA6A}" name="Original Script Name" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{6CD1E5BE-BE71-4E46-9B10-B5E7EC7A2E08}" name="Run By User" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8D7647F2-6793-4883-BE10-614D29E726EB}" name="Order" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{87DCD34E-FC96-4DD0-8734-AF15421982A4}" name="Simplified Script Name" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{313B8C19-4922-44EC-8300-FC839B889845}" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CEB107AC-5D94-4619-B737-91AFD348E2DC}" name="Changed" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A0874E6F-8E55-4E59-8EDD-856191B2FA6A}" name="Original Script Name" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -758,312 +864,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADC88EB-0D15-4452-9F23-EF3ADCBB57B8}">
-  <dimension ref="B3:G18"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D1" s="12"/>
+      <c r="F1"/>
+      <c r="G1" s="1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D2" s="12"/>
+      <c r="F2"/>
+      <c r="G2" s="1"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="C6" s="10">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="G6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2" t="s">
+      <c r="C7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="10">
+        <v>4</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="C16" s="10">
+        <v>6</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="10">
+        <v>9</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="10">
+        <v>10</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="10">
         <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="6"/>
+      <c r="H20"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B4:B20">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
@@ -1073,11 +1273,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168D2C70-AB99-42AD-BFF3-2C13094B0BB7}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6697E1-6CC3-4E1C-9A88-E8518BD48519}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,13 +1327,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1108,50 +1344,50 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
       <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1159,74 +1395,74 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1470,184 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D63068-3BEB-44C9-9201-2F3E7730DF42}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E7360B-42FD-4B5F-AF71-007BB8C1704A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>